<commit_message>
added todos and got double to long conversion
</commit_message>
<xml_diff>
--- a/EducationalScheduler/src/main/resources/sheet.xlsx
+++ b/EducationalScheduler/src/main/resources/sheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomson\VSCode\Scheduler\EducationalScheduler\src\main\resources\"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>Username</t>
   </si>
@@ -63,12 +63,16 @@
   </si>
   <si>
     <t>Current Occupancy</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -414,7 +418,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -422,47 +426,67 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" customWidth="true" width="30.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>81217733</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>8.9128184E7</v>
       </c>
     </row>
   </sheetData>
@@ -478,26 +502,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ensures username is unique
</commit_message>
<xml_diff>
--- a/EducationalScheduler/src/main/resources/sheet.xlsx
+++ b/EducationalScheduler/src/main/resources/sheet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
   <si>
     <t>Student ID</t>
   </si>
@@ -72,6 +72,27 @@
   </si>
   <si>
     <t>7/27/2023</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>12/12/1212</t>
+  </si>
+  <si>
+    <t>notadmin</t>
+  </si>
+  <si>
+    <t>it workssss</t>
+  </si>
+  <si>
+    <t>jack</t>
+  </si>
+  <si>
+    <t>12-23-2222</t>
   </si>
 </sst>
 </file>
@@ -436,7 +457,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E5" sqref="A1:XFD1048576"/>
@@ -490,6 +511,46 @@
       </c>
       <c r="F3" t="n" s="0">
         <v>5.3777259E7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>6.9176879E7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F5" t="n" s="0">
+        <v>8.7999924E7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
comments and timelost constructors
</commit_message>
<xml_diff>
--- a/EducationalScheduler/src/main/resources/sheet.xlsx
+++ b/EducationalScheduler/src/main/resources/sheet.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomson\VSCode\Scheduler\EducationalScheduler\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E4CFB2-5653-4D66-9F53-5851F5CA613A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEBEBE2-6F81-485B-A347-E4411105BA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35130" yWindow="1620" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2235" yWindow="1950" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Account Information" sheetId="1" r:id="rId1"/>
@@ -96,19 +96,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,17 +122,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -454,120 +441,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.7109375"/>
-    <col min="6" max="6" customWidth="true" width="30.7109375"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C2" s="1"/>
-      <c r="E2" s="2"/>
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>53777259</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="F3" s="0">
-        <v>53777259</v>
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>69176879</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="F4" s="0">
-        <v>69176879</v>
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <v>87999924</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="F5" s="0">
-        <v>87999924</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
+      <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="F6" t="n" s="0">
-        <v>9.9153856E7</v>
+      <c r="F5">
+        <v>99153856</v>
       </c>
     </row>
   </sheetData>
@@ -577,30 +560,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="A1:XFD1048576"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.0"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="B1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="B2" t="s" s="0">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Not finalized, full code
</commit_message>
<xml_diff>
--- a/EducationalScheduler/src/main/resources/sheet.xlsx
+++ b/EducationalScheduler/src/main/resources/sheet.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomson\VSCode\Scheduler\EducationalScheduler\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEBEBE2-6F81-485B-A347-E4411105BA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2485B1-5525-41D8-B1CC-EA7F26FD63EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="1950" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3210" yWindow="1710" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Account Information" sheetId="1" r:id="rId1"/>
     <sheet name="Timeslot Information" sheetId="2" r:id="rId2"/>
+    <sheet name="Class Information" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
   <si>
     <t>Username</t>
   </si>
@@ -90,6 +91,141 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Class Name</t>
+  </si>
+  <si>
+    <t>Time Spend</t>
+  </si>
+  <si>
+    <t>Professor</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>Max Occupancy</t>
+  </si>
+  <si>
+    <t>Current Occupancy</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>8:00-9:00</t>
+  </si>
+  <si>
+    <t>Jane Doe</t>
+  </si>
+  <si>
+    <t>A-123</t>
+  </si>
+  <si>
+    <t>Geometry</t>
+  </si>
+  <si>
+    <t>9:00-10:00</t>
+  </si>
+  <si>
+    <t>Kevin Smith</t>
+  </si>
+  <si>
+    <t>A-231</t>
+  </si>
+  <si>
+    <t>Physics</t>
+  </si>
+  <si>
+    <t>10:00-11:00</t>
+  </si>
+  <si>
+    <t>Jennifer Jones</t>
+  </si>
+  <si>
+    <t>B-102</t>
+  </si>
+  <si>
+    <t>Chemistry</t>
+  </si>
+  <si>
+    <t>11:00-12:00</t>
+  </si>
+  <si>
+    <t>David Smith</t>
+  </si>
+  <si>
+    <t>B-204</t>
+  </si>
+  <si>
+    <t>Biology</t>
+  </si>
+  <si>
+    <t>12:00-13:00</t>
+  </si>
+  <si>
+    <t>Eric Huang</t>
+  </si>
+  <si>
+    <t>B-123</t>
+  </si>
+  <si>
+    <t>Philosphy</t>
+  </si>
+  <si>
+    <t>13:00-14:00</t>
+  </si>
+  <si>
+    <t>Vincent Ku</t>
+  </si>
+  <si>
+    <t>Linear Algebra</t>
+  </si>
+  <si>
+    <t>14:00-15:00</t>
+  </si>
+  <si>
+    <t>Joshua Hu</t>
+  </si>
+  <si>
+    <t>Discrete Math</t>
+  </si>
+  <si>
+    <t>15:00-16:00</t>
+  </si>
+  <si>
+    <t>Linda J</t>
+  </si>
+  <si>
+    <t>Calculus</t>
+  </si>
+  <si>
+    <t>16:00-17:00</t>
+  </si>
+  <si>
+    <t>Henry H</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>17:00-18:00</t>
+  </si>
+  <si>
+    <t>Julie J</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>18:00-19:00</t>
+  </si>
+  <si>
+    <t>Jason L</t>
+  </si>
+  <si>
+    <t>A-210</t>
   </si>
 </sst>
 </file>
@@ -125,8 +261,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,7 +699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -590,4 +727,262 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D8198F-5BCB-46DC-8706-938AE1A0D475}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2">
+        <v>12345</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3">
+        <v>12346</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4">
+        <v>12347</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5">
+        <v>12348</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <v>12349</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>12350</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8">
+        <v>12351</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9">
+        <v>12352</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10">
+        <v>12353</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11">
+        <v>12354</v>
+      </c>
+      <c r="D11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12">
+        <v>12355</v>
+      </c>
+      <c r="D12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Timeslot read error fixed
</commit_message>
<xml_diff>
--- a/EducationalScheduler/src/main/resources/sheet.xlsx
+++ b/EducationalScheduler/src/main/resources/sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomson\VSCode\Scheduler\EducationalScheduler\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B794C73E-EE36-4CA7-BB3E-CF931FB4AD04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBDD6EB-13BC-46EA-ADFE-C0ADFD1F11B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29190" yWindow="-540" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31020" yWindow="1410" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Account Information" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="65">
   <si>
     <t>Username</t>
   </si>
@@ -180,6 +180,27 @@
     <t>A-210</t>
   </si>
   <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
     <t>admin</t>
   </si>
   <si>
@@ -189,79 +210,13 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>12/26/2000</t>
-  </si>
-  <si>
-    <t>Monday</t>
-  </si>
-  <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
-    <t>Thursday</t>
-  </si>
-  <si>
-    <t>Friday</t>
-  </si>
-  <si>
-    <t>Saturday</t>
-  </si>
-  <si>
-    <t>Sunday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NULL	,NULL	,NULL	,NULL	,NULL	,NULL	,NULL	,NULL	,NULL	,NULL	,NULL	,NULL	</t>
-  </si>
-  <si>
-    <t>admin2</t>
-  </si>
-  <si>
-    <t>admin2@gmail.com</t>
-  </si>
-  <si>
-    <t>Admin2</t>
+    <t>11/11/1111</t>
   </si>
   <si>
     <t>null,null,null,null,null,null,null,null,null,null,null,null</t>
   </si>
   <si>
-    <t>admin3</t>
-  </si>
-  <si>
-    <t>admin3@gmail.com</t>
-  </si>
-  <si>
-    <t>Admin3</t>
-  </si>
-  <si>
-    <t>admin4</t>
-  </si>
-  <si>
-    <t>admin4@gmail.com</t>
-  </si>
-  <si>
-    <t>Admin4</t>
-  </si>
-  <si>
-    <t>admin5</t>
-  </si>
-  <si>
-    <t>admin5@gmail.com</t>
-  </si>
-  <si>
-    <t>Admin5</t>
-  </si>
-  <si>
-    <t>admin6</t>
-  </si>
-  <si>
-    <t>admin6@gmail.com</t>
-  </si>
-  <si>
-    <t>Admin6</t>
+    <t>null,null,null,null,Biology,Biology,Biology,Biology,Biology,Biology,Biology,Biology</t>
   </si>
 </sst>
 </file>
@@ -615,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F5"/>
+      <selection activeCell="A2" sqref="A2:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,124 +602,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s" s="0">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>55</v>
-      </c>
-      <c r="F2" s="0">
-        <v>19048449</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="0">
-        <v>64</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>64</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>66</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>55</v>
-      </c>
-      <c r="F3" s="0">
-        <v>19082831</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s" s="0">
-        <v>68</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>68</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>69</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>70</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>55</v>
-      </c>
-      <c r="F4" s="0">
-        <v>96830157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>72</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>73</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>55</v>
-      </c>
-      <c r="F5" s="0">
-        <v>16050833</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s" s="0">
-        <v>74</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>74</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>75</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>76</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>55</v>
-      </c>
-      <c r="F6" s="0">
-        <v>53317123</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>77</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>77</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>78</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>79</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>55</v>
-      </c>
-      <c r="F7" t="n" s="0">
-        <v>8.7241263E7</v>
+        <v>62</v>
+      </c>
+      <c r="F2" t="n" s="0">
+        <v>4.8914717E7</v>
       </c>
     </row>
   </sheetData>
@@ -774,10 +629,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I16" sqref="I16:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,181 +645,51 @@
         <v>5</v>
       </c>
       <c r="B1" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="F1" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="G1" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="H1" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="E1" t="s" s="0">
-        <v>59</v>
-      </c>
-      <c r="F1" t="s" s="0">
-        <v>60</v>
-      </c>
-      <c r="G1" t="s" s="0">
-        <v>61</v>
-      </c>
-      <c r="H1" t="s" s="0">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="0">
-        <v>19048449</v>
+    </row>
+    <row r="2">
+      <c r="A2" t="n" s="0">
+        <v>4.8914717E7</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="0">
-        <v>19082831</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="0">
-        <v>96830157</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="0">
-        <v>16050833</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="G5" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="H5" t="s" s="0">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="0">
-        <v>53317123</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n" s="0">
-        <v>8.7241263E7</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="G7" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="H7" t="s" s="0">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -977,7 +702,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
everything works but lowercase class names on del
</commit_message>
<xml_diff>
--- a/EducationalScheduler/src/main/resources/sheet.xlsx
+++ b/EducationalScheduler/src/main/resources/sheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="82">
   <si>
     <t>Username</t>
   </si>
@@ -262,6 +262,12 @@
   </si>
   <si>
     <t>null,null,null,null,Biology,null,null,null,null,null,Java,null</t>
+  </si>
+  <si>
+    <t>English,null,null,null,Biology,null,null,null,null,null,Java,null</t>
+  </si>
+  <si>
+    <t>null,null,null,null,null,null,null,null,null,Python,Java,null</t>
   </si>
 </sst>
 </file>
@@ -854,16 +860,16 @@
         <v>1.4447799E7</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>63</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F5" t="s" s="0">
         <v>63</v>
@@ -932,8 +938,8 @@
       <c r="F2" s="0">
         <v>30</v>
       </c>
-      <c r="G2" s="0">
-        <v>0</v>
+      <c r="G2" s="0" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1139,8 +1145,8 @@
       <c r="F11" s="0">
         <v>25</v>
       </c>
-      <c r="G11" s="0">
-        <v>0</v>
+      <c r="G11" s="0" t="n">
+        <v>2.0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1163,7 +1169,7 @@
         <v>30</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>